<commit_message>
Add IR receiver to schematic
</commit_message>
<xml_diff>
--- a/IR.xlsx
+++ b/IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30e098e8b6e456a9/Documenti/School/FTKL/ir-distance-display/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{ECF9952E-92CE-4948-8C0E-F883940179B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AA7C8AC-F7AE-4514-9808-3DC5C2963401}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{ECF9952E-92CE-4948-8C0E-F883940179B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F5F7189-4F1B-4FC3-99F1-3DC908530A46}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1447,7 +1447,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>